<commit_message>
lab 3.4.1 seems done
</commit_message>
<xml_diff>
--- a/electricity-and-magnetism/3-4-1/data/3-4-1.xlsx
+++ b/electricity-and-magnetism/3-4-1/data/3-4-1.xlsx
@@ -68,7 +68,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -155,6 +155,28 @@
       <left style="thin">
         <color theme="1"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color theme="1"/>
       </right>
@@ -171,6 +193,21 @@
         <color theme="1"/>
       </left>
       <right style="thick">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
         <color theme="1"/>
       </right>
       <top style="thin">
@@ -235,9 +272,6 @@
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -250,9 +284,6 @@
     <xf fontId="0" fillId="0" borderId="3" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="3" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -265,22 +296,26 @@
     <xf fontId="0" fillId="0" borderId="7" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="6" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="7" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="8" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="10" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="5" numFmtId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="8" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="10" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="11" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="12" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="13" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -790,7 +825,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="B6" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="B14" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -817,34 +852,34 @@
       </c>
     </row>
     <row r="3" ht="14.25">
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>0.29999999999999999</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>99</v>
       </c>
     </row>
     <row r="4" ht="14.25">
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>0.59999999999999998</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>185.30000000000001</v>
       </c>
     </row>
     <row r="5" ht="14.25">
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>0.91000000000000003</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>288.60000000000002</v>
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>1.2</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>372.5</v>
       </c>
     </row>
@@ -852,7 +887,7 @@
       <c r="C7" s="1">
         <v>1.5</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>463</v>
       </c>
     </row>
@@ -889,56 +924,56 @@
       </c>
     </row>
     <row r="12" ht="14.25">
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
     </row>
     <row r="13" ht="14.25">
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
     </row>
     <row r="14" ht="14.25">
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
     </row>
     <row r="15" ht="14.25">
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
     </row>
     <row r="16" ht="14.25">
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
     </row>
     <row r="17" ht="14.25">
-      <c r="C17" s="4"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="6" t="s">
+      <c r="C17" s="3"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="G17" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="H17" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="18" ht="14.25">
-      <c r="C18" s="4"/>
-      <c r="D18" s="9" t="s">
+      <c r="C18" s="3"/>
+      <c r="D18" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="10"/>
+      <c r="F18" s="9"/>
       <c r="G18" s="10"/>
       <c r="H18" s="11"/>
     </row>
     <row r="19" ht="14.25">
-      <c r="C19" s="4"/>
-      <c r="D19" s="9">
+      <c r="C19" s="3"/>
+      <c r="D19" s="7">
         <v>0.29999999999999999</v>
       </c>
       <c r="E19" s="12">
@@ -955,7 +990,7 @@
       </c>
     </row>
     <row r="20" ht="14.25">
-      <c r="D20" s="9">
+      <c r="D20" s="7">
         <v>0.59999999999999998</v>
       </c>
       <c r="E20" s="12">
@@ -972,10 +1007,10 @@
       </c>
     </row>
     <row r="21" ht="14.25">
-      <c r="D21" s="9">
+      <c r="D21" s="7">
         <v>0.91000000000000003</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="12" t="s">
         <v>8</v>
       </c>
       <c r="F21" s="12">
@@ -992,7 +1027,7 @@
       <c r="D22" s="14">
         <v>1.2</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="12" t="s">
         <v>9</v>
       </c>
       <c r="F22" s="12">
@@ -1006,10 +1041,10 @@
       </c>
     </row>
     <row r="23" ht="14.25">
-      <c r="D23" s="9">
+      <c r="D23" s="7">
         <v>1.5</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="12" t="s">
         <v>10</v>
       </c>
       <c r="F23" s="12">
@@ -1023,7 +1058,7 @@
       </c>
     </row>
     <row r="24" ht="14.25">
-      <c r="D24" s="9">
+      <c r="D24" s="7">
         <v>1.8100000000000001</v>
       </c>
       <c r="E24" s="12">
@@ -1040,7 +1075,7 @@
       </c>
     </row>
     <row r="25" ht="14.25">
-      <c r="D25" s="9">
+      <c r="D25" s="7">
         <v>2.2000000000000002</v>
       </c>
       <c r="E25" s="12">
@@ -1057,7 +1092,7 @@
       </c>
     </row>
     <row r="26" ht="14.25">
-      <c r="D26" s="9">
+      <c r="D26" s="7">
         <v>2.6000000000000001</v>
       </c>
       <c r="E26" s="12">
@@ -1090,11 +1125,11 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E18:H18"/>
+    <mergeCell ref="E18:G18"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>